<commit_message>
add rel paths and txt export
</commit_message>
<xml_diff>
--- a/data/wiki_cultures.xlsx
+++ b/data/wiki_cultures.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1261D-09C8-4BE1-9F4D-B16904CDFD37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,7 +319,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,16 +348,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -619,35 +667,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -655,10 +705,10 @@
       <c r="A2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -666,10 +716,10 @@
       <c r="A3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -677,10 +727,10 @@
       <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -688,10 +738,10 @@
       <c r="A5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -699,10 +749,10 @@
       <c r="A6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -710,7 +760,7 @@
       <c r="A7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
@@ -721,10 +771,10 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -732,10 +782,10 @@
       <c r="A9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -743,10 +793,10 @@
       <c r="A10" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -754,10 +804,10 @@
       <c r="A11" t="s">
         <v>75</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -765,13 +815,13 @@
       <c r="A12" t="s">
         <v>76</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F12" t="s">
@@ -782,13 +832,13 @@
       <c r="A13" t="s">
         <v>76</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F13" t="s">
@@ -799,13 +849,13 @@
       <c r="A14" t="s">
         <v>76</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F14" t="s">
@@ -816,7 +866,7 @@
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -824,7 +874,7 @@
       <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -832,10 +882,10 @@
       <c r="A17" t="s">
         <v>75</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -843,10 +893,10 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -854,13 +904,13 @@
       <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="7" t="s">
         <v>72</v>
       </c>
       <c r="F19" t="s">
@@ -871,13 +921,13 @@
       <c r="A20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F20" t="s">
@@ -888,7 +938,7 @@
       <c r="A21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D21" t="s">
@@ -899,10 +949,10 @@
       <c r="A22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -910,13 +960,13 @@
       <c r="A23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F23" t="s">
@@ -927,10 +977,10 @@
       <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F24" t="s">
@@ -941,10 +991,10 @@
       <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -952,10 +1002,10 @@
       <c r="A26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -963,10 +1013,10 @@
       <c r="A27" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F27" t="s">
@@ -977,10 +1027,10 @@
       <c r="A28" t="s">
         <v>75</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -988,13 +1038,13 @@
       <c r="A29" t="s">
         <v>76</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="7" t="s">
         <v>45</v>
       </c>
       <c r="F29" t="s">
@@ -1005,10 +1055,10 @@
       <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1016,10 +1066,10 @@
       <c r="A31" t="s">
         <v>76</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="7" t="s">
         <v>78</v>
       </c>
       <c r="F31" t="s">
@@ -1030,10 +1080,10 @@
       <c r="A32" t="s">
         <v>76</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F32" t="s">
@@ -1044,10 +1094,10 @@
       <c r="A33" t="s">
         <v>75</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1055,10 +1105,10 @@
       <c r="A34" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D34" t="s">
@@ -1069,10 +1119,10 @@
       <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1080,7 +1130,7 @@
       <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1088,13 +1138,13 @@
       <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="7" t="s">
         <v>59</v>
       </c>
       <c r="F37" t="s">
@@ -1105,14 +1155,22 @@
       <c r="A38" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A59">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add date of retrieval and fix title-language error
</commit_message>
<xml_diff>
--- a/data/wiki_cultures.xlsx
+++ b/data/wiki_cultures.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1261D-09C8-4BE1-9F4D-B16904CDFD37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2E80B2-0190-4331-A4B4-FC6938D7FD9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,17 +361,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -670,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1001,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>42</v>
@@ -1036,7 +1026,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>45</v>
@@ -1078,7 +1068,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>50</v>
@@ -1136,7 +1126,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>59</v>
@@ -1164,10 +1154,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A59">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new descriptions in wiki_cultures
</commit_message>
<xml_diff>
--- a/data/wiki_cultures.xlsx
+++ b/data/wiki_cultures.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2E80B2-0190-4331-A4B4-FC6938D7FD9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A47CC8-5C83-4F8C-8632-89475C283C86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,18 +223,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>{"de": "Fundstellen des Clactonien", "en": "Clactonian sites"}</t>
-  </si>
-  <si>
-    <t>{"en": "Sites of the Fauresmith industry"}</t>
-  </si>
-  <si>
-    <t>{"en": "Emiran sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Szeletien", "en": "Szeletian sites"}</t>
-  </si>
-  <si>
     <t>Micoquian</t>
   </si>
   <si>
@@ -259,34 +247,46 @@
     <t>Fauresmith</t>
   </si>
   <si>
-    <t>{"de": "Fundstellen der la Quina Kultur", "en": "La Quina sites"}</t>
-  </si>
-  <si>
-    <t>{"en": "Ahmarian sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Châtelperronien", "en": "Châtelperronian sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen der Howieson's Poort Industrie", "en": "Howiesons Poort sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Stillbaai", "en": "Stillbaai sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Gravettien", "en": "Gravettian sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Micoquien", "en": "Micoquian sites"}</t>
-  </si>
-  <si>
-    <t>{"de": "Fundstellen des Atérien", "en": "Aterian sites"}</t>
-  </si>
-  <si>
     <t>road_culture</t>
   </si>
   <si>
     <t>use</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Atérien Fundstellen aus der ROAD Datenbank", "en": "Selected Aterian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Micoquien Fundstellen aus der ROAD Datenbank", "en": "Selected Micoquian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Gravettien Fundstellen aus der ROAD Datenbank", "en": "Selected Gravettian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Still Bay Fundstellen aus der ROAD Datenbank", "en": "Selected Still Bay sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Howiesonspoort Fundstellen aus der ROAD Datenbank", "en": "Selected Howiesonspoort sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Châtelperronien Fundstellen aus der ROAD Datenbank", "en": "Selected Châtelperronian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Ahmarien Fundstellen aus der ROAD Datenbank", "en": "Selected Ahmarian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte La Quina Fundstellen aus der ROAD Datenbank", "en": "Selected La Quina sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Clactionien Fundstellen aus der ROAD Datenbank", "en": "Selected Clactionian sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Fauresmith Fundstellen aus der ROAD Datenbank", "en": "Selected Fauresmith sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Emiran Fundstellen aus der ROAD Datenbank", "en": "Selected Emiran sites from the ROAD Database"}</t>
+  </si>
+  <si>
+    <t>{"de": "Ausgewählte Szeletien Fundstellen aus der ROAD Datenbank", "en": "Selected Szeletian sites from the ROAD Database"}</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>64</v>
@@ -685,7 +685,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>66</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>2</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>16</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -815,12 +815,12 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
@@ -829,15 +829,15 @@
         <v>20</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>22</v>
@@ -849,12 +849,12 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>23</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>24</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>25</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>27</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>29</v>
@@ -901,15 +901,15 @@
         <v>29</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>30</v>
@@ -918,15 +918,15 @@
         <v>31</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>32</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>33</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>35</v>
@@ -957,15 +957,15 @@
         <v>36</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>37</v>
@@ -974,12 +974,12 @@
         <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>38</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>40</v>
@@ -1001,21 +1001,21 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>43</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>45</v>
@@ -1038,12 +1038,12 @@
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>47</v>
@@ -1054,21 +1054,21 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>50</v>
@@ -1077,12 +1077,12 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>51</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>53</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>55</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>56</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>59</v>
@@ -1138,12 +1138,12 @@
         <v>59</v>
       </c>
       <c r="F37" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>61</v>

</xml_diff>